<commit_message>
Added correct data for decile UE gained
</commit_message>
<xml_diff>
--- a/Decile UE Gained.xlsx
+++ b/Decile UE Gained.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GGPC\Desktop\INFO281-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72560503-DDC9-4D45-BBA1-D31D9BF6B23E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3794CD2A-F9C8-45D4-8E9F-E1639DC7CFB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -953,7 +953,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>11</v>
       </c>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>11</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>11</v>
       </c>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>12</v>
       </c>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>12</v>
       </c>
@@ -2603,7 +2603,7 @@
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>12</v>
       </c>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>13</v>
       </c>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
         <v>13</v>
       </c>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>13</v>
       </c>
@@ -3923,7 +3923,7 @@
       </c>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>11</v>
       </c>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="K110" s="1"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="6">
         <v>11</v>
       </c>
@@ -4583,7 +4583,7 @@
       </c>
       <c r="K120" s="1"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="6">
         <v>11</v>
       </c>
@@ -4913,7 +4913,7 @@
       </c>
       <c r="K130" s="1"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="6">
         <v>12</v>
       </c>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="K140" s="1"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="6">
         <v>12</v>
       </c>
@@ -5573,7 +5573,7 @@
       </c>
       <c r="K150" s="1"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="6">
         <v>12</v>
       </c>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="K160" s="1"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="6">
         <v>13</v>
       </c>
@@ -6233,7 +6233,7 @@
       </c>
       <c r="K170" s="1"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="6">
         <v>13</v>
       </c>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="K180" s="1"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="6">
         <v>13</v>
       </c>
@@ -6893,7 +6893,7 @@
       </c>
       <c r="K190" s="1"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="6">
         <v>11</v>
       </c>
@@ -7223,7 +7223,7 @@
       </c>
       <c r="K200" s="1"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="6">
         <v>11</v>
       </c>
@@ -7553,7 +7553,7 @@
       </c>
       <c r="K210" s="1"/>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="6">
         <v>11</v>
       </c>
@@ -7883,7 +7883,7 @@
       </c>
       <c r="K220" s="1"/>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="6">
         <v>12</v>
       </c>
@@ -8213,7 +8213,7 @@
       </c>
       <c r="K230" s="1"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="6">
         <v>12</v>
       </c>
@@ -8543,7 +8543,7 @@
       </c>
       <c r="K240" s="1"/>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="6">
         <v>12</v>
       </c>
@@ -8873,7 +8873,7 @@
       </c>
       <c r="K250" s="1"/>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="6">
         <v>13</v>
       </c>
@@ -9203,7 +9203,7 @@
       </c>
       <c r="K260" s="1"/>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="6">
         <v>13</v>
       </c>
@@ -9533,7 +9533,7 @@
       </c>
       <c r="K270" s="1"/>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="6">
         <v>13</v>
       </c>
@@ -9863,7 +9863,7 @@
       </c>
       <c r="K280" s="1"/>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="6">
         <v>11</v>
       </c>
@@ -10193,7 +10193,7 @@
       </c>
       <c r="K290" s="1"/>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="6">
         <v>11</v>
       </c>
@@ -10523,7 +10523,7 @@
       </c>
       <c r="K300" s="1"/>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" s="6">
         <v>11</v>
       </c>
@@ -10853,7 +10853,7 @@
       </c>
       <c r="K310" s="1"/>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" s="6">
         <v>12</v>
       </c>
@@ -11183,7 +11183,7 @@
       </c>
       <c r="K320" s="1"/>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" s="6">
         <v>12</v>
       </c>
@@ -11513,7 +11513,7 @@
       </c>
       <c r="K330" s="1"/>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" s="6">
         <v>12</v>
       </c>
@@ -12538,6 +12538,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K361" xr:uid="{7E2B6FF3-4F73-4E2F-A7AA-FFBDE5C80143}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="13"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="University Entrance"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="3">
       <filters>
         <filter val="2018"/>

</xml_diff>